<commit_message>
Updated TIPSY model and reference data.
</commit_message>
<xml_diff>
--- a/references/TIPSY/Cutblock_species.xlsx
+++ b/references/TIPSY/Cutblock_species.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userc\Documents\wood-budget\wood-budget\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userc\Documents\wood-budget\wood-budget\references\TIPSY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B2EB9D-C0FE-4700-80C9-1F4A23E4C77B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF033A45-9CC4-4F5B-8CD8-6108D015CE2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3050" yWindow="1080" windowWidth="14400" windowHeight="7880" xr2:uid="{71EC3472-C6D1-4679-ABE5-2CEA0D488550}"/>
+    <workbookView xWindow="13930" yWindow="4080" windowWidth="14400" windowHeight="7360" xr2:uid="{71EC3472-C6D1-4679-ABE5-2CEA0D488550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>48353488/L\SwPl\834-0/12\he,by\$I06</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Density (SPA)</t>
+  </si>
+  <si>
+    <t>Q_diam</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -478,11 +481,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -509,15 +551,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,481 +877,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F24C2D-A8EA-48BB-B846-308E4269E932}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="A1:M21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="11" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="N1" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="34">
+        <v>23.381</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11">
+      <c r="E2" s="10"/>
+      <c r="F2" s="11">
         <v>63</v>
       </c>
-      <c r="F2" s="11">
+      <c r="G2" s="11">
         <v>37</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12">
-        <v>143</v>
-      </c>
+      <c r="H2" s="11"/>
       <c r="I2" s="12">
         <v>143</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
+        <v>143</v>
+      </c>
+      <c r="K2" s="13">
         <v>26.1</v>
       </c>
-      <c r="K2" s="13">
+      <c r="L2" s="13">
         <v>21.6</v>
       </c>
-      <c r="L2" s="28">
+      <c r="M2" s="27">
         <v>12.8</v>
       </c>
-      <c r="M2" s="31">
+      <c r="N2" s="30">
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="34">
+        <v>21.774000000000001</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11">
         <v>50.1</v>
       </c>
-      <c r="F3" s="11">
+      <c r="G3" s="11">
         <v>49.9</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12">
-        <v>143</v>
-      </c>
+      <c r="H3" s="11"/>
       <c r="I3" s="12">
         <v>143</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
+        <v>143</v>
+      </c>
+      <c r="K3" s="13">
         <v>21.6</v>
       </c>
-      <c r="K3" s="13">
+      <c r="L3" s="13">
         <v>26.1</v>
       </c>
-      <c r="L3" s="28">
+      <c r="M3" s="27">
         <v>13.7</v>
       </c>
-      <c r="M3" s="31">
+      <c r="N3" s="30">
         <v>967</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="34">
+        <v>21.375</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11">
+      <c r="E4" s="10"/>
+      <c r="F4" s="11">
         <v>94</v>
       </c>
-      <c r="F4" s="11">
+      <c r="G4" s="11">
         <v>6</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12">
-        <v>123</v>
-      </c>
+      <c r="H4" s="11"/>
       <c r="I4" s="12">
         <v>123</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
+        <v>123</v>
+      </c>
+      <c r="K4" s="13">
         <v>21.8</v>
       </c>
-      <c r="K4" s="13">
+      <c r="L4" s="13">
         <v>14.9</v>
       </c>
-      <c r="L4" s="28">
+      <c r="M4" s="27">
         <v>14.8</v>
       </c>
-      <c r="M4" s="31">
+      <c r="N4" s="30">
         <v>1161</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="34">
+        <v>25.995000000000001</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11">
+      <c r="E5" s="10"/>
+      <c r="F5" s="11">
         <v>94</v>
       </c>
-      <c r="F5" s="11">
+      <c r="G5" s="11">
         <v>6</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12">
-        <v>148</v>
-      </c>
+      <c r="H5" s="11"/>
       <c r="I5" s="12">
         <v>148</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
+        <v>148</v>
+      </c>
+      <c r="K5" s="13">
         <v>26.6</v>
       </c>
-      <c r="K5" s="13">
+      <c r="L5" s="13">
         <v>31.8</v>
       </c>
-      <c r="L5" s="28">
+      <c r="M5" s="27">
         <v>17.8</v>
       </c>
-      <c r="M5" s="31">
+      <c r="N5" s="30">
         <v>817</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="34">
+        <v>27</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="11">
+      <c r="E6" s="10"/>
+      <c r="F6" s="11">
         <v>100</v>
       </c>
-      <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="12">
+      <c r="H6" s="11"/>
+      <c r="I6" s="12">
         <v>148</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13">
+      <c r="J6" s="12"/>
+      <c r="K6" s="13">
         <v>27.6</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="28">
+      <c r="L6" s="13"/>
+      <c r="M6" s="27">
         <v>18.7</v>
       </c>
-      <c r="M6" s="31">
+      <c r="N6" s="30">
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="35">
+        <v>19.29</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="21"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="22">
+      <c r="E7" s="21"/>
+      <c r="F7" s="22">
         <v>100</v>
       </c>
-      <c r="F7" s="22"/>
       <c r="G7" s="22"/>
-      <c r="H7" s="23">
+      <c r="H7" s="22"/>
+      <c r="I7" s="23">
         <v>143</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24">
+      <c r="J7" s="23"/>
+      <c r="K7" s="24">
         <v>18.600000000000001</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="29">
+      <c r="L7" s="24"/>
+      <c r="M7" s="28">
         <v>11.3</v>
       </c>
-      <c r="M7" s="32">
+      <c r="N7" s="31">
         <v>570</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="M8">
-        <f>AVERAGE(M2:M7)</f>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <f>AVERAGE(B2:B7)</f>
+        <v>23.135833333333334</v>
+      </c>
+      <c r="K8">
+        <f>AVERAGE(K2:K7,L2:L5)</f>
+        <v>23.669999999999998</v>
+      </c>
+      <c r="N8">
+        <f>AVERAGE(N2:N7)</f>
         <v>780.83333333333337</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B12" s="5">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C12" s="5">
         <v>63</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>50.1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>13.7</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>12.8</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>143</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>26.1</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>143</v>
       </c>
-      <c r="I12" s="6">
+      <c r="J12" s="6">
         <v>21.6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B13" s="5">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C13" s="5">
         <v>49.9</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>94</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>14.8</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
         <v>143</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>26.1</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>143</v>
       </c>
-      <c r="I13" s="6">
+      <c r="J13" s="6">
         <v>21.6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B14" s="5">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>94</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>17.8</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
         <v>123</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>14.9</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>123</v>
       </c>
-      <c r="I14" s="6">
+      <c r="J14" s="6">
         <v>21.8</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B15" s="5">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C15" s="5">
         <v>6</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>100</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>18.7</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
         <v>148</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>31.8</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>148</v>
       </c>
-      <c r="I15" s="6">
+      <c r="J15" s="6">
         <v>26.6</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B16" s="5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C16" s="5">
         <v>0</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>100</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>11.3</v>
       </c>
-      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1">
         <v>148</v>
       </c>
-      <c r="I16" s="6">
+      <c r="J16" s="6">
         <v>27.6</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="5">
+    <row r="17" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C17" s="5">
         <v>0</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>37</v>
       </c>
-      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1">
         <v>143</v>
       </c>
-      <c r="I17" s="6">
+      <c r="J17" s="6">
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="7">
-        <f>AVERAGE(B12:B17)</f>
+    <row r="18" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="7">
+        <f>AVERAGE(C12:C17)</f>
         <v>20.816666666666666</v>
       </c>
-      <c r="C18" s="8">
-        <f t="shared" ref="C18:I18" si="0">AVERAGE(C12:C17)</f>
+      <c r="D18" s="8">
+        <f t="shared" ref="D18:J18" si="0">AVERAGE(D12:D17)</f>
         <v>79.183333333333337</v>
       </c>
-      <c r="D18" s="25">
+      <c r="E18" s="25">
         <f t="shared" si="0"/>
         <v>15.26</v>
       </c>
-      <c r="E18" s="8">
+      <c r="F18" s="8">
         <f t="shared" si="0"/>
         <v>12.8</v>
       </c>
-      <c r="F18" s="25">
+      <c r="G18" s="25">
         <f t="shared" si="0"/>
         <v>139.25</v>
       </c>
-      <c r="G18" s="25">
+      <c r="H18" s="25">
         <f t="shared" si="0"/>
         <v>24.725000000000001</v>
       </c>
-      <c r="H18" s="8">
+      <c r="I18" s="8">
         <f t="shared" si="0"/>
         <v>141.33333333333334</v>
       </c>
-      <c r="I18" s="9">
+      <c r="J18" s="9">
         <f t="shared" si="0"/>
         <v>22.966666666666665</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D19" t="s">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="G19" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="26"/>
+      <c r="H19" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>